<commit_message>
changes to gantt chart and acceptance tests
</commit_message>
<xml_diff>
--- a/report/assets/gantt-diagram.xlsx
+++ b/report/assets/gantt-diagram.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EFB55D-5D38-4B36-A890-3D1F73ACDA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB35390D-4CD3-4BF1-8044-503CEE5B631D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16245" yWindow="-24120" windowWidth="57840" windowHeight="24240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Sample phase title block</t>
-  </si>
-  <si>
-    <t>This is an empty row</t>
   </si>
   <si>
     <t>This row marks the end of the Project Schedule. DO NOT enter anything in this row. 
@@ -219,22 +216,10 @@
     <t>Sprint 1</t>
   </si>
   <si>
-    <t>Sprint 1 Review</t>
-  </si>
-  <si>
     <t>Sprint 2</t>
   </si>
   <si>
-    <t>Sprint 2 Review</t>
-  </si>
-  <si>
     <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
-    <t>Sprint 3 Review</t>
   </si>
   <si>
     <t>Background Research</t>
@@ -249,25 +234,7 @@
     <t>Testing Strategy &amp; Results</t>
   </si>
   <si>
-    <t>Testing Strategy</t>
-  </si>
-  <si>
-    <t>Test Results</t>
-  </si>
-  <si>
-    <t>Noteworthy Test Results</t>
-  </si>
-  <si>
     <t>Evalutaion</t>
-  </si>
-  <si>
-    <t>Positives</t>
-  </si>
-  <si>
-    <t>Reflection on Project</t>
-  </si>
-  <si>
-    <t>Negatives</t>
   </si>
   <si>
     <t>Evaluation</t>
@@ -280,9 +247,6 @@
   </si>
   <si>
     <t>Sprint 3 Preparation</t>
-  </si>
-  <si>
-    <t>Task 9</t>
   </si>
   <si>
     <t>Task 8</t>
@@ -302,6 +266,33 @@
   <si>
     <t>Task 11</t>
   </si>
+  <si>
+    <t>Implementation Cut Off</t>
+  </si>
+  <si>
+    <t>Overflow Time</t>
+  </si>
+  <si>
+    <t>Benchmark Tests</t>
+  </si>
+  <si>
+    <t>Acceptance Tests</t>
+  </si>
+  <si>
+    <t>Test Evaluation</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Reflection</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
 </sst>
 </file>
 
@@ -317,7 +308,7 @@
     <numFmt numFmtId="168" formatCode="d"/>
     <numFmt numFmtId="169" formatCode="d\ mmm\ yyyy"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,8 +538,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="50">
+  <fills count="51">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,6 +837,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -1103,7 +1116,7 @@
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1396,26 +1409,6 @@
     <xf numFmtId="168" fontId="9" fillId="7" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="19"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="19" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="49" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1427,6 +1420,39 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="49" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="19" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="11" fillId="50" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="50" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="19" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1998,13 +2024,13 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:HD52"/>
+  <dimension ref="A1:HD51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="7" topLeftCell="BZ38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="7" topLeftCell="I17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2043,8 +2069,10 @@
     <col min="150" max="150" width="1.6640625" bestFit="1" customWidth="1"/>
     <col min="151" max="151" width="2.21875" bestFit="1" customWidth="1"/>
     <col min="152" max="152" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="153" max="174" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="175" max="176" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="153" max="173" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="2.44140625" customWidth="1"/>
+    <col min="175" max="175" width="1.6640625" style="115" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="1.6640625" bestFit="1" customWidth="1"/>
     <col min="177" max="177" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="178" max="178" width="1.6640625" bestFit="1" customWidth="1"/>
     <col min="179" max="179" width="2.21875" bestFit="1" customWidth="1"/>
@@ -2061,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -2070,7 +2098,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="54"/>
       <c r="L1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="Q1">
         <v>21</v>
@@ -2081,342 +2109,358 @@
         <v>1</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="55"/>
-      <c r="BN2" s="111"/>
-      <c r="BO2" s="111"/>
-      <c r="BP2" s="111"/>
-      <c r="BQ2" s="111"/>
-      <c r="BR2" s="111"/>
-      <c r="BS2" s="111"/>
-      <c r="GX2" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="GY2" s="104"/>
-      <c r="GZ2" s="104"/>
-      <c r="HA2" s="104"/>
-      <c r="HB2" s="104"/>
-      <c r="HC2" s="104"/>
-      <c r="HD2" s="104"/>
+      <c r="BN2" s="114"/>
+      <c r="BO2" s="114"/>
+      <c r="BP2" s="114"/>
+      <c r="BQ2" s="114"/>
+      <c r="BR2" s="114"/>
+      <c r="BS2" s="114"/>
+      <c r="FS2" s="120" t="s">
+        <v>64</v>
+      </c>
+      <c r="FT2" s="120"/>
+      <c r="FU2" s="120"/>
+      <c r="FV2" s="120"/>
+      <c r="FW2" s="120"/>
+      <c r="FX2" s="120"/>
+      <c r="FY2" s="120"/>
+      <c r="FZ2" s="120"/>
+      <c r="GA2" s="120"/>
+      <c r="GB2" s="120"/>
+      <c r="GC2" s="120"/>
+      <c r="GD2" s="120"/>
+      <c r="GE2" s="120"/>
+      <c r="GF2" s="120"/>
+      <c r="GX2" s="119" t="s">
+        <v>36</v>
+      </c>
+      <c r="GY2" s="119"/>
+      <c r="GZ2" s="119"/>
+      <c r="HA2" s="119"/>
+      <c r="HB2" s="119"/>
+      <c r="HC2" s="119"/>
+      <c r="HD2" s="119"/>
     </row>
     <row r="3" spans="1:212" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="105" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="106"/>
-      <c r="E3" s="110">
+        <v>28</v>
+      </c>
+      <c r="C3" s="111" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="112"/>
+      <c r="E3" s="113">
         <v>44851</v>
       </c>
-      <c r="F3" s="110"/>
+      <c r="F3" s="113"/>
     </row>
     <row r="4" spans="1:212" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="105" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="106"/>
+      <c r="C4" s="111" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="112"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="107">
+      <c r="I4" s="108">
         <f>I5</f>
         <v>44851</v>
       </c>
-      <c r="J4" s="108"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="108"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="107">
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="110"/>
+      <c r="P4" s="108">
         <f>P5</f>
         <v>44858</v>
       </c>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="108"/>
-      <c r="S4" s="108"/>
-      <c r="T4" s="108"/>
-      <c r="U4" s="108"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="107">
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+      <c r="V4" s="110"/>
+      <c r="W4" s="108">
         <f>W5</f>
         <v>44865</v>
       </c>
-      <c r="X4" s="108"/>
-      <c r="Y4" s="108"/>
-      <c r="Z4" s="108"/>
-      <c r="AA4" s="108"/>
-      <c r="AB4" s="108"/>
-      <c r="AC4" s="109"/>
-      <c r="AD4" s="107">
+      <c r="X4" s="109"/>
+      <c r="Y4" s="109"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
+      <c r="AB4" s="109"/>
+      <c r="AC4" s="110"/>
+      <c r="AD4" s="108">
         <f>AD5</f>
         <v>44872</v>
       </c>
-      <c r="AE4" s="108"/>
-      <c r="AF4" s="108"/>
-      <c r="AG4" s="108"/>
-      <c r="AH4" s="108"/>
-      <c r="AI4" s="108"/>
-      <c r="AJ4" s="109"/>
-      <c r="AK4" s="107">
+      <c r="AE4" s="109"/>
+      <c r="AF4" s="109"/>
+      <c r="AG4" s="109"/>
+      <c r="AH4" s="109"/>
+      <c r="AI4" s="109"/>
+      <c r="AJ4" s="110"/>
+      <c r="AK4" s="108">
         <f>AK5</f>
         <v>44879</v>
       </c>
-      <c r="AL4" s="108"/>
-      <c r="AM4" s="108"/>
-      <c r="AN4" s="108"/>
-      <c r="AO4" s="108"/>
-      <c r="AP4" s="108"/>
-      <c r="AQ4" s="109"/>
-      <c r="AR4" s="107">
+      <c r="AL4" s="109"/>
+      <c r="AM4" s="109"/>
+      <c r="AN4" s="109"/>
+      <c r="AO4" s="109"/>
+      <c r="AP4" s="109"/>
+      <c r="AQ4" s="110"/>
+      <c r="AR4" s="108">
         <f>AR5</f>
         <v>44886</v>
       </c>
-      <c r="AS4" s="108"/>
-      <c r="AT4" s="108"/>
-      <c r="AU4" s="108"/>
-      <c r="AV4" s="108"/>
-      <c r="AW4" s="108"/>
-      <c r="AX4" s="109"/>
-      <c r="AY4" s="107">
+      <c r="AS4" s="109"/>
+      <c r="AT4" s="109"/>
+      <c r="AU4" s="109"/>
+      <c r="AV4" s="109"/>
+      <c r="AW4" s="109"/>
+      <c r="AX4" s="110"/>
+      <c r="AY4" s="108">
         <f>AY5</f>
         <v>44893</v>
       </c>
-      <c r="AZ4" s="108"/>
-      <c r="BA4" s="108"/>
-      <c r="BB4" s="108"/>
-      <c r="BC4" s="108"/>
-      <c r="BD4" s="108"/>
-      <c r="BE4" s="109"/>
-      <c r="BF4" s="107">
+      <c r="AZ4" s="109"/>
+      <c r="BA4" s="109"/>
+      <c r="BB4" s="109"/>
+      <c r="BC4" s="109"/>
+      <c r="BD4" s="109"/>
+      <c r="BE4" s="110"/>
+      <c r="BF4" s="108">
         <f>BF5</f>
         <v>44900</v>
       </c>
-      <c r="BG4" s="108"/>
-      <c r="BH4" s="108"/>
-      <c r="BI4" s="108"/>
-      <c r="BJ4" s="108"/>
-      <c r="BK4" s="108"/>
-      <c r="BL4" s="109"/>
-      <c r="BM4" s="107">
+      <c r="BG4" s="109"/>
+      <c r="BH4" s="109"/>
+      <c r="BI4" s="109"/>
+      <c r="BJ4" s="109"/>
+      <c r="BK4" s="109"/>
+      <c r="BL4" s="110"/>
+      <c r="BM4" s="108">
         <f>BM5</f>
         <v>44907</v>
       </c>
-      <c r="BN4" s="108"/>
-      <c r="BO4" s="108"/>
-      <c r="BP4" s="108"/>
-      <c r="BQ4" s="108"/>
-      <c r="BR4" s="108"/>
-      <c r="BS4" s="109"/>
-      <c r="BT4" s="107">
+      <c r="BN4" s="109"/>
+      <c r="BO4" s="109"/>
+      <c r="BP4" s="109"/>
+      <c r="BQ4" s="109"/>
+      <c r="BR4" s="109"/>
+      <c r="BS4" s="110"/>
+      <c r="BT4" s="108">
         <f>BT5</f>
         <v>44914</v>
       </c>
-      <c r="BU4" s="108"/>
-      <c r="BV4" s="108"/>
-      <c r="BW4" s="108"/>
-      <c r="BX4" s="108"/>
-      <c r="BY4" s="108"/>
-      <c r="BZ4" s="109"/>
-      <c r="CA4" s="107">
+      <c r="BU4" s="109"/>
+      <c r="BV4" s="109"/>
+      <c r="BW4" s="109"/>
+      <c r="BX4" s="109"/>
+      <c r="BY4" s="109"/>
+      <c r="BZ4" s="110"/>
+      <c r="CA4" s="108">
         <f>CA5</f>
         <v>44921</v>
       </c>
-      <c r="CB4" s="108"/>
-      <c r="CC4" s="108"/>
-      <c r="CD4" s="108"/>
-      <c r="CE4" s="108"/>
-      <c r="CF4" s="108"/>
-      <c r="CG4" s="109"/>
-      <c r="CH4" s="107">
+      <c r="CB4" s="109"/>
+      <c r="CC4" s="109"/>
+      <c r="CD4" s="109"/>
+      <c r="CE4" s="109"/>
+      <c r="CF4" s="109"/>
+      <c r="CG4" s="110"/>
+      <c r="CH4" s="108">
         <f>CH5</f>
         <v>44928</v>
       </c>
-      <c r="CI4" s="108"/>
-      <c r="CJ4" s="108"/>
-      <c r="CK4" s="108"/>
-      <c r="CL4" s="108"/>
-      <c r="CM4" s="108"/>
-      <c r="CN4" s="109"/>
-      <c r="CO4" s="107">
+      <c r="CI4" s="109"/>
+      <c r="CJ4" s="109"/>
+      <c r="CK4" s="109"/>
+      <c r="CL4" s="109"/>
+      <c r="CM4" s="109"/>
+      <c r="CN4" s="110"/>
+      <c r="CO4" s="108">
         <f>CO5</f>
         <v>44935</v>
       </c>
-      <c r="CP4" s="108"/>
-      <c r="CQ4" s="108"/>
-      <c r="CR4" s="108"/>
-      <c r="CS4" s="108"/>
-      <c r="CT4" s="108"/>
-      <c r="CU4" s="109"/>
-      <c r="CV4" s="107">
+      <c r="CP4" s="109"/>
+      <c r="CQ4" s="109"/>
+      <c r="CR4" s="109"/>
+      <c r="CS4" s="109"/>
+      <c r="CT4" s="109"/>
+      <c r="CU4" s="110"/>
+      <c r="CV4" s="108">
         <f>CV5</f>
         <v>44942</v>
       </c>
-      <c r="CW4" s="108"/>
-      <c r="CX4" s="108"/>
-      <c r="CY4" s="108"/>
-      <c r="CZ4" s="108"/>
-      <c r="DA4" s="108"/>
-      <c r="DB4" s="109"/>
-      <c r="DC4" s="107">
+      <c r="CW4" s="109"/>
+      <c r="CX4" s="109"/>
+      <c r="CY4" s="109"/>
+      <c r="CZ4" s="109"/>
+      <c r="DA4" s="109"/>
+      <c r="DB4" s="110"/>
+      <c r="DC4" s="108">
         <f t="shared" ref="DC4" si="0">DC5</f>
         <v>44949</v>
       </c>
-      <c r="DD4" s="108"/>
-      <c r="DE4" s="108"/>
-      <c r="DF4" s="108"/>
-      <c r="DG4" s="108"/>
-      <c r="DH4" s="108"/>
-      <c r="DI4" s="109"/>
-      <c r="DJ4" s="107">
+      <c r="DD4" s="109"/>
+      <c r="DE4" s="109"/>
+      <c r="DF4" s="109"/>
+      <c r="DG4" s="109"/>
+      <c r="DH4" s="109"/>
+      <c r="DI4" s="110"/>
+      <c r="DJ4" s="108">
         <f t="shared" ref="DJ4" si="1">DJ5</f>
         <v>44956</v>
       </c>
-      <c r="DK4" s="108"/>
-      <c r="DL4" s="108"/>
-      <c r="DM4" s="108"/>
-      <c r="DN4" s="108"/>
-      <c r="DO4" s="108"/>
-      <c r="DP4" s="109"/>
-      <c r="DQ4" s="107">
+      <c r="DK4" s="109"/>
+      <c r="DL4" s="109"/>
+      <c r="DM4" s="109"/>
+      <c r="DN4" s="109"/>
+      <c r="DO4" s="109"/>
+      <c r="DP4" s="110"/>
+      <c r="DQ4" s="108">
         <f t="shared" ref="DQ4" si="2">DQ5</f>
         <v>44963</v>
       </c>
-      <c r="DR4" s="108"/>
-      <c r="DS4" s="108"/>
-      <c r="DT4" s="108"/>
-      <c r="DU4" s="108"/>
-      <c r="DV4" s="108"/>
-      <c r="DW4" s="109"/>
-      <c r="DX4" s="107">
+      <c r="DR4" s="109"/>
+      <c r="DS4" s="109"/>
+      <c r="DT4" s="109"/>
+      <c r="DU4" s="109"/>
+      <c r="DV4" s="109"/>
+      <c r="DW4" s="110"/>
+      <c r="DX4" s="108">
         <f t="shared" ref="DX4" si="3">DX5</f>
         <v>44970</v>
       </c>
-      <c r="DY4" s="108"/>
-      <c r="DZ4" s="108"/>
-      <c r="EA4" s="108"/>
-      <c r="EB4" s="108"/>
-      <c r="EC4" s="108"/>
-      <c r="ED4" s="109"/>
-      <c r="EE4" s="107">
+      <c r="DY4" s="109"/>
+      <c r="DZ4" s="109"/>
+      <c r="EA4" s="109"/>
+      <c r="EB4" s="109"/>
+      <c r="EC4" s="109"/>
+      <c r="ED4" s="110"/>
+      <c r="EE4" s="108">
         <f t="shared" ref="EE4" si="4">EE5</f>
         <v>44977</v>
       </c>
-      <c r="EF4" s="108"/>
-      <c r="EG4" s="108"/>
-      <c r="EH4" s="108"/>
-      <c r="EI4" s="108"/>
-      <c r="EJ4" s="108"/>
-      <c r="EK4" s="109"/>
-      <c r="EL4" s="107">
+      <c r="EF4" s="109"/>
+      <c r="EG4" s="109"/>
+      <c r="EH4" s="109"/>
+      <c r="EI4" s="109"/>
+      <c r="EJ4" s="109"/>
+      <c r="EK4" s="110"/>
+      <c r="EL4" s="108">
         <f t="shared" ref="EL4" si="5">EL5</f>
         <v>44984</v>
       </c>
-      <c r="EM4" s="108"/>
-      <c r="EN4" s="108"/>
-      <c r="EO4" s="108"/>
-      <c r="EP4" s="108"/>
-      <c r="EQ4" s="108"/>
-      <c r="ER4" s="109"/>
-      <c r="ES4" s="107">
+      <c r="EM4" s="109"/>
+      <c r="EN4" s="109"/>
+      <c r="EO4" s="109"/>
+      <c r="EP4" s="109"/>
+      <c r="EQ4" s="109"/>
+      <c r="ER4" s="110"/>
+      <c r="ES4" s="108">
         <f t="shared" ref="ES4" si="6">ES5</f>
         <v>44991</v>
       </c>
-      <c r="ET4" s="108"/>
-      <c r="EU4" s="108"/>
-      <c r="EV4" s="108"/>
-      <c r="EW4" s="108"/>
-      <c r="EX4" s="108"/>
-      <c r="EY4" s="109"/>
-      <c r="EZ4" s="107">
+      <c r="ET4" s="109"/>
+      <c r="EU4" s="109"/>
+      <c r="EV4" s="109"/>
+      <c r="EW4" s="109"/>
+      <c r="EX4" s="109"/>
+      <c r="EY4" s="110"/>
+      <c r="EZ4" s="108">
         <f t="shared" ref="EZ4" si="7">EZ5</f>
         <v>44998</v>
       </c>
-      <c r="FA4" s="108"/>
-      <c r="FB4" s="108"/>
-      <c r="FC4" s="108"/>
-      <c r="FD4" s="108"/>
-      <c r="FE4" s="108"/>
-      <c r="FF4" s="109"/>
-      <c r="FG4" s="107">
+      <c r="FA4" s="109"/>
+      <c r="FB4" s="109"/>
+      <c r="FC4" s="109"/>
+      <c r="FD4" s="109"/>
+      <c r="FE4" s="109"/>
+      <c r="FF4" s="110"/>
+      <c r="FG4" s="108">
         <f t="shared" ref="FG4" si="8">FG5</f>
         <v>45005</v>
       </c>
-      <c r="FH4" s="108"/>
-      <c r="FI4" s="108"/>
-      <c r="FJ4" s="108"/>
-      <c r="FK4" s="108"/>
-      <c r="FL4" s="108"/>
-      <c r="FM4" s="109"/>
-      <c r="FN4" s="107">
+      <c r="FH4" s="109"/>
+      <c r="FI4" s="109"/>
+      <c r="FJ4" s="109"/>
+      <c r="FK4" s="109"/>
+      <c r="FL4" s="109"/>
+      <c r="FM4" s="110"/>
+      <c r="FN4" s="108">
         <f t="shared" ref="FN4" si="9">FN5</f>
         <v>45012</v>
       </c>
-      <c r="FO4" s="108"/>
-      <c r="FP4" s="108"/>
-      <c r="FQ4" s="108"/>
-      <c r="FR4" s="108"/>
-      <c r="FS4" s="108"/>
-      <c r="FT4" s="109"/>
-      <c r="FU4" s="107">
+      <c r="FO4" s="109"/>
+      <c r="FP4" s="109"/>
+      <c r="FQ4" s="109"/>
+      <c r="FR4" s="109"/>
+      <c r="FS4" s="109"/>
+      <c r="FT4" s="110"/>
+      <c r="FU4" s="108">
         <f t="shared" ref="FU4" si="10">FU5</f>
         <v>45019</v>
       </c>
-      <c r="FV4" s="108"/>
-      <c r="FW4" s="108"/>
-      <c r="FX4" s="108"/>
-      <c r="FY4" s="108"/>
-      <c r="FZ4" s="108"/>
-      <c r="GA4" s="109"/>
-      <c r="GB4" s="107">
+      <c r="FV4" s="109"/>
+      <c r="FW4" s="109"/>
+      <c r="FX4" s="109"/>
+      <c r="FY4" s="109"/>
+      <c r="FZ4" s="109"/>
+      <c r="GA4" s="110"/>
+      <c r="GB4" s="108">
         <f t="shared" ref="GB4" si="11">GB5</f>
         <v>45026</v>
       </c>
-      <c r="GC4" s="108"/>
-      <c r="GD4" s="108"/>
-      <c r="GE4" s="108"/>
-      <c r="GF4" s="108"/>
-      <c r="GG4" s="108"/>
-      <c r="GH4" s="109"/>
-      <c r="GI4" s="107">
+      <c r="GC4" s="109"/>
+      <c r="GD4" s="109"/>
+      <c r="GE4" s="109"/>
+      <c r="GF4" s="109"/>
+      <c r="GG4" s="109"/>
+      <c r="GH4" s="110"/>
+      <c r="GI4" s="108">
         <f t="shared" ref="GI4" si="12">GI5</f>
         <v>45033</v>
       </c>
-      <c r="GJ4" s="108"/>
-      <c r="GK4" s="108"/>
-      <c r="GL4" s="108"/>
-      <c r="GM4" s="108"/>
-      <c r="GN4" s="108"/>
-      <c r="GO4" s="109"/>
-      <c r="GP4" s="107">
+      <c r="GJ4" s="109"/>
+      <c r="GK4" s="109"/>
+      <c r="GL4" s="109"/>
+      <c r="GM4" s="109"/>
+      <c r="GN4" s="109"/>
+      <c r="GO4" s="110"/>
+      <c r="GP4" s="108">
         <f t="shared" ref="GP4" si="13">GP5</f>
         <v>45040</v>
       </c>
-      <c r="GQ4" s="108"/>
-      <c r="GR4" s="108"/>
-      <c r="GS4" s="108"/>
-      <c r="GT4" s="108"/>
-      <c r="GU4" s="108"/>
-      <c r="GV4" s="109"/>
-      <c r="GW4" s="107">
+      <c r="GQ4" s="109"/>
+      <c r="GR4" s="109"/>
+      <c r="GS4" s="109"/>
+      <c r="GT4" s="109"/>
+      <c r="GU4" s="109"/>
+      <c r="GV4" s="110"/>
+      <c r="GW4" s="108">
         <f t="shared" ref="GW4" si="14">GW5</f>
         <v>45047</v>
       </c>
-      <c r="GX4" s="108"/>
-      <c r="GY4" s="108"/>
-      <c r="GZ4" s="108"/>
-      <c r="HA4" s="108"/>
-      <c r="HB4" s="108"/>
-      <c r="HC4" s="109"/>
+      <c r="GX4" s="109"/>
+      <c r="GY4" s="109"/>
+      <c r="GZ4" s="109"/>
+      <c r="HA4" s="109"/>
+      <c r="HB4" s="109"/>
+      <c r="HC4" s="110"/>
     </row>
     <row r="5" spans="1:212" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
@@ -3092,7 +3136,7 @@
         <f t="shared" ref="FR5" si="94">FQ5+1</f>
         <v>45016</v>
       </c>
-      <c r="FS5" s="71">
+      <c r="FS5" s="116">
         <f t="shared" ref="FS5" si="95">FR5+1</f>
         <v>45017</v>
       </c>
@@ -3246,23 +3290,23 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="10" t="str">
         <f t="shared" ref="I6" si="132">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -3928,7 +3972,7 @@
         <f t="shared" si="141"/>
         <v>F</v>
       </c>
-      <c r="FS6" s="10" t="str">
+      <c r="FS6" s="117" t="str">
         <f t="shared" si="141"/>
         <v>S</v>
       </c>
@@ -4253,7 +4297,7 @@
       <c r="FP7" s="30"/>
       <c r="FQ7" s="30"/>
       <c r="FR7" s="30"/>
-      <c r="FS7" s="30"/>
+      <c r="FS7" s="118"/>
       <c r="FT7" s="30"/>
       <c r="FU7" s="30"/>
       <c r="FV7" s="30"/>
@@ -4296,7 +4340,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="15"/>
@@ -4304,7 +4348,7 @@
       <c r="F8" s="57"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="str">
-        <f t="shared" ref="H8:H49" si="143">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H48" si="143">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="30"/>
@@ -4473,7 +4517,7 @@
       <c r="FP8" s="30"/>
       <c r="FQ8" s="30"/>
       <c r="FR8" s="30"/>
-      <c r="FS8" s="30"/>
+      <c r="FS8" s="118"/>
       <c r="FT8" s="30"/>
       <c r="FU8" s="30"/>
       <c r="FV8" s="30"/>
@@ -4516,10 +4560,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
@@ -4702,7 +4746,7 @@
       <c r="FP9" s="30"/>
       <c r="FQ9" s="30"/>
       <c r="FR9" s="30"/>
-      <c r="FS9" s="30"/>
+      <c r="FS9" s="118"/>
       <c r="FT9" s="30"/>
       <c r="FU9" s="30"/>
       <c r="FV9" s="30"/>
@@ -4745,10 +4789,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
@@ -4932,7 +4976,7 @@
       <c r="FP10" s="30"/>
       <c r="FQ10" s="30"/>
       <c r="FR10" s="30"/>
-      <c r="FS10" s="30"/>
+      <c r="FS10" s="118"/>
       <c r="FT10" s="30"/>
       <c r="FU10" s="30"/>
       <c r="FV10" s="30"/>
@@ -4973,10 +5017,10 @@
     <row r="11" spans="1:212" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="34"/>
       <c r="B11" s="49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D11" s="16">
         <v>1</v>
@@ -5160,7 +5204,7 @@
       <c r="FP11" s="30"/>
       <c r="FQ11" s="30"/>
       <c r="FR11" s="30"/>
-      <c r="FS11" s="30"/>
+      <c r="FS11" s="118"/>
       <c r="FT11" s="30"/>
       <c r="FU11" s="30"/>
       <c r="FV11" s="30"/>
@@ -5201,10 +5245,10 @@
     <row r="12" spans="1:212" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="34"/>
       <c r="B12" s="49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="16">
         <v>1</v>
@@ -5388,7 +5432,7 @@
       <c r="FP12" s="30"/>
       <c r="FQ12" s="30"/>
       <c r="FR12" s="30"/>
-      <c r="FS12" s="30"/>
+      <c r="FS12" s="118"/>
       <c r="FT12" s="30"/>
       <c r="FU12" s="30"/>
       <c r="FV12" s="30"/>
@@ -5429,10 +5473,10 @@
     <row r="13" spans="1:212" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="34"/>
       <c r="B13" s="49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="77" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="16">
         <f>AVERAGE(D9:D12)</f>
@@ -5617,7 +5661,7 @@
       <c r="FP13" s="30"/>
       <c r="FQ13" s="30"/>
       <c r="FR13" s="30"/>
-      <c r="FS13" s="30"/>
+      <c r="FS13" s="118"/>
       <c r="FT13" s="30"/>
       <c r="FU13" s="30"/>
       <c r="FV13" s="30"/>
@@ -5660,7 +5704,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="18"/>
@@ -5837,7 +5881,7 @@
       <c r="FP14" s="30"/>
       <c r="FQ14" s="30"/>
       <c r="FR14" s="30"/>
-      <c r="FS14" s="30"/>
+      <c r="FS14" s="118"/>
       <c r="FT14" s="30"/>
       <c r="FU14" s="30"/>
       <c r="FV14" s="30"/>
@@ -5878,10 +5922,10 @@
     <row r="15" spans="1:212" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="35"/>
       <c r="B15" s="50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D15" s="19">
         <v>1</v>
@@ -6062,7 +6106,7 @@
       <c r="FP15" s="30"/>
       <c r="FQ15" s="30"/>
       <c r="FR15" s="30"/>
-      <c r="FS15" s="30"/>
+      <c r="FS15" s="118"/>
       <c r="FT15" s="30"/>
       <c r="FU15" s="30"/>
       <c r="FV15" s="30"/>
@@ -6103,10 +6147,10 @@
     <row r="16" spans="1:212" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="35"/>
       <c r="B16" s="50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="19">
         <v>1</v>
@@ -6290,7 +6334,7 @@
       <c r="FP16" s="30"/>
       <c r="FQ16" s="30"/>
       <c r="FR16" s="30"/>
-      <c r="FS16" s="30"/>
+      <c r="FS16" s="118"/>
       <c r="FT16" s="30"/>
       <c r="FU16" s="30"/>
       <c r="FV16" s="30"/>
@@ -6331,10 +6375,10 @@
     <row r="17" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34"/>
       <c r="B17" s="50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
@@ -6518,7 +6562,7 @@
       <c r="FP17" s="30"/>
       <c r="FQ17" s="30"/>
       <c r="FR17" s="30"/>
-      <c r="FS17" s="30"/>
+      <c r="FS17" s="118"/>
       <c r="FT17" s="30"/>
       <c r="FU17" s="30"/>
       <c r="FV17" s="30"/>
@@ -6559,10 +6603,10 @@
     <row r="18" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="34"/>
       <c r="B18" s="50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="19">
         <v>1</v>
@@ -6745,7 +6789,7 @@
       <c r="FP18" s="30"/>
       <c r="FQ18" s="30"/>
       <c r="FR18" s="30"/>
-      <c r="FS18" s="30"/>
+      <c r="FS18" s="118"/>
       <c r="FT18" s="30"/>
       <c r="FU18" s="30"/>
       <c r="FV18" s="30"/>
@@ -6786,7 +6830,7 @@
     <row r="19" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="34"/>
       <c r="B19" s="50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="19"/>
@@ -6963,7 +7007,7 @@
       <c r="FP19" s="30"/>
       <c r="FQ19" s="30"/>
       <c r="FR19" s="30"/>
-      <c r="FS19" s="30"/>
+      <c r="FS19" s="118"/>
       <c r="FT19" s="30"/>
       <c r="FU19" s="30"/>
       <c r="FV19" s="30"/>
@@ -7004,10 +7048,10 @@
     <row r="20" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="34"/>
       <c r="B20" s="50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="78" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="19">
         <f>AVERAGE(D15:D18)</f>
@@ -7192,7 +7236,7 @@
       <c r="FP20" s="30"/>
       <c r="FQ20" s="30"/>
       <c r="FR20" s="30"/>
-      <c r="FS20" s="30"/>
+      <c r="FS20" s="118"/>
       <c r="FT20" s="30"/>
       <c r="FU20" s="30"/>
       <c r="FV20" s="30"/>
@@ -7235,7 +7279,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="45"/>
       <c r="D21" s="21"/>
@@ -7412,7 +7456,7 @@
       <c r="FP21" s="30"/>
       <c r="FQ21" s="30"/>
       <c r="FR21" s="30"/>
-      <c r="FS21" s="30"/>
+      <c r="FS21" s="118"/>
       <c r="FT21" s="30"/>
       <c r="FU21" s="30"/>
       <c r="FV21" s="30"/>
@@ -7453,10 +7497,10 @@
     <row r="22" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="34"/>
       <c r="B22" s="51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="22">
         <v>1</v>
@@ -7640,7 +7684,7 @@
       <c r="FP22" s="30"/>
       <c r="FQ22" s="30"/>
       <c r="FR22" s="30"/>
-      <c r="FS22" s="30"/>
+      <c r="FS22" s="118"/>
       <c r="FT22" s="30"/>
       <c r="FU22" s="30"/>
       <c r="FV22" s="30"/>
@@ -7681,13 +7725,13 @@
     <row r="23" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="34"/>
       <c r="B23" s="51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="22">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E23" s="64">
         <v>44907</v>
@@ -7867,7 +7911,7 @@
       <c r="FP23" s="30"/>
       <c r="FQ23" s="30"/>
       <c r="FR23" s="30"/>
-      <c r="FS23" s="30"/>
+      <c r="FS23" s="118"/>
       <c r="FT23" s="30"/>
       <c r="FU23" s="30"/>
       <c r="FV23" s="30"/>
@@ -7908,7 +7952,7 @@
     <row r="24" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="34"/>
       <c r="B24" s="51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="46"/>
       <c r="D24" s="22"/>
@@ -8085,7 +8129,7 @@
       <c r="FP24" s="30"/>
       <c r="FQ24" s="30"/>
       <c r="FR24" s="30"/>
-      <c r="FS24" s="30"/>
+      <c r="FS24" s="118"/>
       <c r="FT24" s="30"/>
       <c r="FU24" s="30"/>
       <c r="FV24" s="30"/>
@@ -8126,14 +8170,14 @@
     <row r="25" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="34"/>
       <c r="B25" s="51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="79" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="22">
         <f>AVERAGE(D22:D23,D16:D18,D9:D12)</f>
-        <v>0.97222222222222221</v>
+        <v>1</v>
       </c>
       <c r="E25" s="64">
         <f>E9</f>
@@ -8313,7 +8357,7 @@
       <c r="FP25" s="30"/>
       <c r="FQ25" s="30"/>
       <c r="FR25" s="30"/>
-      <c r="FS25" s="30"/>
+      <c r="FS25" s="118"/>
       <c r="FT25" s="30"/>
       <c r="FU25" s="30"/>
       <c r="FV25" s="30"/>
@@ -8356,7 +8400,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="47"/>
       <c r="D26" s="24"/>
@@ -8533,7 +8577,7 @@
       <c r="FP26" s="30"/>
       <c r="FQ26" s="30"/>
       <c r="FR26" s="30"/>
-      <c r="FS26" s="30"/>
+      <c r="FS26" s="118"/>
       <c r="FT26" s="30"/>
       <c r="FU26" s="30"/>
       <c r="FV26" s="30"/>
@@ -8574,13 +8618,13 @@
     <row r="27" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
       <c r="B27" s="52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D27" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="67">
         <v>44909</v>
@@ -8757,7 +8801,7 @@
       <c r="FP27" s="30"/>
       <c r="FQ27" s="30"/>
       <c r="FR27" s="30"/>
-      <c r="FS27" s="30"/>
+      <c r="FS27" s="118"/>
       <c r="FT27" s="30"/>
       <c r="FU27" s="30"/>
       <c r="FV27" s="30"/>
@@ -8798,26 +8842,25 @@
     <row r="28" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="34"/>
       <c r="B28" s="52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="67">
-        <f t="shared" ref="E28:E35" si="144">F27+1</f>
+        <f t="shared" ref="E28:E30" si="144">F27+1</f>
         <v>44912</v>
       </c>
       <c r="F28" s="67">
-        <f>E28+Q1</f>
-        <v>44933</v>
+        <v>44943</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="13">
         <f t="shared" si="143"/>
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="I28" s="30"/>
       <c r="J28" s="30"/>
@@ -8985,7 +9028,7 @@
       <c r="FP28" s="30"/>
       <c r="FQ28" s="30"/>
       <c r="FR28" s="30"/>
-      <c r="FS28" s="30"/>
+      <c r="FS28" s="118"/>
       <c r="FT28" s="30"/>
       <c r="FU28" s="30"/>
       <c r="FV28" s="30"/>
@@ -9029,24 +9072,21 @@
         <v>17</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D29" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="67">
-        <f t="shared" si="144"/>
-        <v>44934</v>
+        <f>F28+1</f>
+        <v>44944</v>
       </c>
       <c r="F29" s="67">
-        <f>E29+3</f>
-        <v>44937</v>
+        <f>E29+5</f>
+        <v>44949</v>
       </c>
       <c r="G29" s="13"/>
-      <c r="H29" s="13">
-        <f t="shared" si="143"/>
-        <v>4</v>
-      </c>
+      <c r="H29" s="13"/>
       <c r="I29" s="30"/>
       <c r="J29" s="30"/>
       <c r="K29" s="30"/>
@@ -9213,7 +9253,7 @@
       <c r="FP29" s="30"/>
       <c r="FQ29" s="30"/>
       <c r="FR29" s="30"/>
-      <c r="FS29" s="30"/>
+      <c r="FS29" s="118"/>
       <c r="FT29" s="30"/>
       <c r="FU29" s="30"/>
       <c r="FV29" s="30"/>
@@ -9257,21 +9297,23 @@
         <v>18</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D30" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="67">
         <f t="shared" si="144"/>
-        <v>44938</v>
+        <v>44950</v>
       </c>
       <c r="F30" s="67">
-        <f>E30+3</f>
-        <v>44941</v>
+        <v>44979</v>
       </c>
       <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="H30" s="13">
+        <f t="shared" si="143"/>
+        <v>30</v>
+      </c>
       <c r="I30" s="30"/>
       <c r="J30" s="30"/>
       <c r="K30" s="30"/>
@@ -9438,7 +9480,7 @@
       <c r="FP30" s="30"/>
       <c r="FQ30" s="30"/>
       <c r="FR30" s="30"/>
-      <c r="FS30" s="30"/>
+      <c r="FS30" s="118"/>
       <c r="FT30" s="30"/>
       <c r="FU30" s="30"/>
       <c r="FV30" s="30"/>
@@ -9479,27 +9521,24 @@
     <row r="31" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="34"/>
       <c r="B31" s="52" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D31" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="67">
-        <f t="shared" si="144"/>
-        <v>44942</v>
+        <f>F30+1</f>
+        <v>44980</v>
       </c>
       <c r="F31" s="67">
-        <f>E31+Q1</f>
-        <v>44963</v>
+        <f>E31+3</f>
+        <v>44983</v>
       </c>
       <c r="G31" s="13"/>
-      <c r="H31" s="13">
-        <f t="shared" si="143"/>
-        <v>22</v>
-      </c>
+      <c r="H31" s="13"/>
       <c r="I31" s="30"/>
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
@@ -9666,7 +9705,7 @@
       <c r="FP31" s="30"/>
       <c r="FQ31" s="30"/>
       <c r="FR31" s="30"/>
-      <c r="FS31" s="30"/>
+      <c r="FS31" s="118"/>
       <c r="FT31" s="30"/>
       <c r="FU31" s="30"/>
       <c r="FV31" s="30"/>
@@ -9707,26 +9746,25 @@
     <row r="32" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="34"/>
       <c r="B32" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="48" t="s">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="C32" s="80" t="s">
+        <v>48</v>
       </c>
       <c r="D32" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="67">
-        <f t="shared" si="144"/>
-        <v>44964</v>
+        <f>F31+1</f>
+        <v>44984</v>
       </c>
       <c r="F32" s="67">
-        <f>E32+3</f>
-        <v>44967</v>
+        <v>45012</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13">
         <f t="shared" si="143"/>
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="I32" s="30"/>
       <c r="J32" s="30"/>
@@ -9894,7 +9932,7 @@
       <c r="FP32" s="30"/>
       <c r="FQ32" s="30"/>
       <c r="FR32" s="30"/>
-      <c r="FS32" s="30"/>
+      <c r="FS32" s="118"/>
       <c r="FT32" s="30"/>
       <c r="FU32" s="30"/>
       <c r="FV32" s="30"/>
@@ -9935,21 +9973,21 @@
     <row r="33" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="34"/>
       <c r="B33" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="48" t="s">
-        <v>68</v>
+        <v>58</v>
+      </c>
+      <c r="C33" s="80" t="s">
+        <v>65</v>
       </c>
       <c r="D33" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="67">
-        <f t="shared" si="144"/>
-        <v>44968</v>
+        <f>F32+1</f>
+        <v>45013</v>
       </c>
       <c r="F33" s="67">
         <f>E33+3</f>
-        <v>44971</v>
+        <v>45016</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
@@ -10119,7 +10157,7 @@
       <c r="FP33" s="30"/>
       <c r="FQ33" s="30"/>
       <c r="FR33" s="30"/>
-      <c r="FS33" s="30"/>
+      <c r="FS33" s="118"/>
       <c r="FT33" s="30"/>
       <c r="FU33" s="30"/>
       <c r="FV33" s="30"/>
@@ -10160,27 +10198,24 @@
     <row r="34" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="34"/>
       <c r="B34" s="52" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C34" s="80" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D34" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="67">
-        <f t="shared" si="144"/>
-        <v>44972</v>
+        <f>F33+1</f>
+        <v>45017</v>
       </c>
       <c r="F34" s="67">
-        <f>E34+Q1</f>
-        <v>44993</v>
+        <f>E34+7</f>
+        <v>45024</v>
       </c>
       <c r="G34" s="13"/>
-      <c r="H34" s="13">
-        <f t="shared" si="143"/>
-        <v>22</v>
-      </c>
+      <c r="H34" s="13"/>
       <c r="I34" s="30"/>
       <c r="J34" s="30"/>
       <c r="K34" s="30"/>
@@ -10347,7 +10382,7 @@
       <c r="FP34" s="30"/>
       <c r="FQ34" s="30"/>
       <c r="FR34" s="30"/>
-      <c r="FS34" s="30"/>
+      <c r="FS34" s="118"/>
       <c r="FT34" s="30"/>
       <c r="FU34" s="30"/>
       <c r="FV34" s="30"/>
@@ -10386,31 +10421,27 @@
       <c r="HC34" s="30"/>
     </row>
     <row r="35" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="34" t="s">
-        <v>12</v>
-      </c>
+      <c r="A35" s="34"/>
       <c r="B35" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="80" t="s">
-        <v>53</v>
+        <v>63</v>
+      </c>
+      <c r="C35" s="81" t="s">
+        <v>41</v>
       </c>
       <c r="D35" s="25">
-        <v>0</v>
+        <f>AVERAGE(D27:D34)</f>
+        <v>1</v>
       </c>
       <c r="E35" s="67">
-        <f t="shared" si="144"/>
-        <v>44994</v>
+        <f>E27</f>
+        <v>44909</v>
       </c>
       <c r="F35" s="67">
-        <f>E35+3</f>
-        <v>44997</v>
+        <f>F34</f>
+        <v>45024</v>
       </c>
       <c r="G35" s="13"/>
-      <c r="H35" s="13">
-        <f t="shared" si="143"/>
-        <v>4</v>
-      </c>
+      <c r="H35" s="13"/>
       <c r="I35" s="30"/>
       <c r="J35" s="30"/>
       <c r="K35" s="30"/>
@@ -10577,7 +10608,7 @@
       <c r="FP35" s="30"/>
       <c r="FQ35" s="30"/>
       <c r="FR35" s="30"/>
-      <c r="FS35" s="30"/>
+      <c r="FS35" s="118"/>
       <c r="FT35" s="30"/>
       <c r="FU35" s="30"/>
       <c r="FV35" s="30"/>
@@ -10617,23 +10648,13 @@
     </row>
     <row r="36" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="34"/>
-      <c r="B36" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="80" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="25">
-        <v>0</v>
-      </c>
-      <c r="E36" s="67">
-        <f>F35+1</f>
-        <v>44998</v>
-      </c>
-      <c r="F36" s="67">
-        <f>E36+7</f>
-        <v>45005</v>
-      </c>
+      <c r="B36" s="83" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="82"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="30"/>
@@ -10802,7 +10823,7 @@
       <c r="FP36" s="30"/>
       <c r="FQ36" s="30"/>
       <c r="FR36" s="30"/>
-      <c r="FS36" s="30"/>
+      <c r="FS36" s="118"/>
       <c r="FT36" s="30"/>
       <c r="FU36" s="30"/>
       <c r="FV36" s="30"/>
@@ -10842,23 +10863,22 @@
     </row>
     <row r="37" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="34"/>
-      <c r="B37" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="25">
-        <f>AVERAGE(D27:D36)</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="67">
-        <f>E28</f>
-        <v>44912</v>
-      </c>
-      <c r="F37" s="67">
-        <f>F36</f>
-        <v>45005</v>
+      <c r="B37" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="89">
+        <v>0.33</v>
+      </c>
+      <c r="E37" s="90">
+        <f>F35+1</f>
+        <v>45025</v>
+      </c>
+      <c r="F37" s="90">
+        <f>E37+3</f>
+        <v>45028</v>
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
@@ -11028,7 +11048,7 @@
       <c r="FP37" s="30"/>
       <c r="FQ37" s="30"/>
       <c r="FR37" s="30"/>
-      <c r="FS37" s="30"/>
+      <c r="FS37" s="118"/>
       <c r="FT37" s="30"/>
       <c r="FU37" s="30"/>
       <c r="FV37" s="30"/>
@@ -11068,13 +11088,23 @@
     </row>
     <row r="38" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="34"/>
-      <c r="B38" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="82"/>
-      <c r="D38" s="84"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
+      <c r="B38" s="87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="89">
+        <v>0.25</v>
+      </c>
+      <c r="E38" s="90">
+        <f>F37+1</f>
+        <v>45029</v>
+      </c>
+      <c r="F38" s="90">
+        <f>E38+3</f>
+        <v>45032</v>
+      </c>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="30"/>
@@ -11243,7 +11273,7 @@
       <c r="FP38" s="30"/>
       <c r="FQ38" s="30"/>
       <c r="FR38" s="30"/>
-      <c r="FS38" s="30"/>
+      <c r="FS38" s="118"/>
       <c r="FT38" s="30"/>
       <c r="FU38" s="30"/>
       <c r="FV38" s="30"/>
@@ -11284,21 +11314,21 @@
     <row r="39" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="34"/>
       <c r="B39" s="87" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C39" s="88" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D39" s="89">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="E39" s="90">
-        <f>F37+1</f>
-        <v>45006</v>
+        <f>F38+1</f>
+        <v>45033</v>
       </c>
       <c r="F39" s="90">
-        <f>E39+7</f>
-        <v>45013</v>
+        <f>E39+2</f>
+        <v>45035</v>
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
@@ -11468,7 +11498,7 @@
       <c r="FP39" s="30"/>
       <c r="FQ39" s="30"/>
       <c r="FR39" s="30"/>
-      <c r="FS39" s="30"/>
+      <c r="FS39" s="118"/>
       <c r="FT39" s="30"/>
       <c r="FU39" s="30"/>
       <c r="FV39" s="30"/>
@@ -11509,21 +11539,22 @@
     <row r="40" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="34"/>
       <c r="B40" s="87" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="88" t="s">
-        <v>59</v>
+        <v>17</v>
+      </c>
+      <c r="C40" s="86" t="s">
+        <v>52</v>
       </c>
       <c r="D40" s="89">
-        <v>0</v>
+        <f>AVERAGE(D37:D39)</f>
+        <v>0.31</v>
       </c>
       <c r="E40" s="90">
-        <f>F39+1</f>
-        <v>45014</v>
+        <f>E37</f>
+        <v>45025</v>
       </c>
       <c r="F40" s="90">
-        <f>E40+5</f>
-        <v>45019</v>
+        <f>F39</f>
+        <v>45035</v>
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
@@ -11693,7 +11724,7 @@
       <c r="FP40" s="30"/>
       <c r="FQ40" s="30"/>
       <c r="FR40" s="30"/>
-      <c r="FS40" s="30"/>
+      <c r="FS40" s="118"/>
       <c r="FT40" s="30"/>
       <c r="FU40" s="30"/>
       <c r="FV40" s="30"/>
@@ -11733,23 +11764,13 @@
     </row>
     <row r="41" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="34"/>
-      <c r="B41" s="87" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="88" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="89">
-        <v>0</v>
-      </c>
-      <c r="E41" s="90">
-        <f>F40+1</f>
-        <v>45020</v>
-      </c>
-      <c r="F41" s="90">
-        <f>E41+3</f>
-        <v>45023</v>
-      </c>
+      <c r="B41" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="91"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="93"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
       <c r="I41" s="30"/>
@@ -11918,7 +11939,7 @@
       <c r="FP41" s="30"/>
       <c r="FQ41" s="30"/>
       <c r="FR41" s="30"/>
-      <c r="FS41" s="30"/>
+      <c r="FS41" s="118"/>
       <c r="FT41" s="30"/>
       <c r="FU41" s="30"/>
       <c r="FV41" s="30"/>
@@ -11958,23 +11979,22 @@
     </row>
     <row r="42" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="34"/>
-      <c r="B42" s="87" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="89">
-        <f>AVERAGE(D39:D41)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="90">
-        <f>E39</f>
-        <v>45006</v>
-      </c>
-      <c r="F42" s="90">
-        <f>F41</f>
-        <v>45023</v>
+      <c r="B42" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="96">
+        <v>0.35</v>
+      </c>
+      <c r="E42" s="97">
+        <f>F40+1</f>
+        <v>45036</v>
+      </c>
+      <c r="F42" s="97">
+        <f>E42+2</f>
+        <v>45038</v>
       </c>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
@@ -12144,7 +12164,7 @@
       <c r="FP42" s="30"/>
       <c r="FQ42" s="30"/>
       <c r="FR42" s="30"/>
-      <c r="FS42" s="30"/>
+      <c r="FS42" s="118"/>
       <c r="FT42" s="30"/>
       <c r="FU42" s="30"/>
       <c r="FV42" s="30"/>
@@ -12184,13 +12204,23 @@
     </row>
     <row r="43" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="34"/>
-      <c r="B43" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="91"/>
-      <c r="D43" s="92"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
+      <c r="B43" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="96">
+        <v>0.15</v>
+      </c>
+      <c r="E43" s="97">
+        <f>F42+1</f>
+        <v>45039</v>
+      </c>
+      <c r="F43" s="97">
+        <f>E43+2</f>
+        <v>45041</v>
+      </c>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
       <c r="I43" s="30"/>
@@ -12359,7 +12389,7 @@
       <c r="FP43" s="30"/>
       <c r="FQ43" s="30"/>
       <c r="FR43" s="30"/>
-      <c r="FS43" s="30"/>
+      <c r="FS43" s="118"/>
       <c r="FT43" s="30"/>
       <c r="FU43" s="30"/>
       <c r="FV43" s="30"/>
@@ -12400,21 +12430,21 @@
     <row r="44" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="34"/>
       <c r="B44" s="98" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C44" s="99" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D44" s="96">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E44" s="97">
-        <f>F42+1</f>
-        <v>45024</v>
+        <f>F43+1</f>
+        <v>45042</v>
       </c>
       <c r="F44" s="97">
-        <f>E44+3</f>
-        <v>45027</v>
+        <f>E44+2</f>
+        <v>45044</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
@@ -12584,7 +12614,7 @@
       <c r="FP44" s="30"/>
       <c r="FQ44" s="30"/>
       <c r="FR44" s="30"/>
-      <c r="FS44" s="30"/>
+      <c r="FS44" s="118"/>
       <c r="FT44" s="30"/>
       <c r="FU44" s="30"/>
       <c r="FV44" s="30"/>
@@ -12625,21 +12655,21 @@
     <row r="45" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="34"/>
       <c r="B45" s="98" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C45" s="99" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D45" s="96">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E45" s="97">
         <f>F44+1</f>
-        <v>45028</v>
+        <v>45045</v>
       </c>
       <c r="F45" s="97">
-        <f>E45+3</f>
-        <v>45031</v>
+        <f>E45+1</f>
+        <v>45046</v>
       </c>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
@@ -12809,7 +12839,7 @@
       <c r="FP45" s="30"/>
       <c r="FQ45" s="30"/>
       <c r="FR45" s="30"/>
-      <c r="FS45" s="30"/>
+      <c r="FS45" s="118"/>
       <c r="FT45" s="30"/>
       <c r="FU45" s="30"/>
       <c r="FV45" s="30"/>
@@ -12850,21 +12880,22 @@
     <row r="46" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34"/>
       <c r="B46" s="98" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="99" t="s">
-        <v>63</v>
+        <v>18</v>
+      </c>
+      <c r="C46" s="95" t="s">
+        <v>54</v>
       </c>
       <c r="D46" s="96">
-        <v>0</v>
+        <f>AVERAGE(D42:D45)</f>
+        <v>0.21250000000000002</v>
       </c>
       <c r="E46" s="97">
-        <f>F45+1</f>
-        <v>45032</v>
+        <f>E42</f>
+        <v>45036</v>
       </c>
       <c r="F46" s="97">
-        <f>E46+5</f>
-        <v>45037</v>
+        <f>F45</f>
+        <v>45046</v>
       </c>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
@@ -13034,7 +13065,7 @@
       <c r="FP46" s="30"/>
       <c r="FQ46" s="30"/>
       <c r="FR46" s="30"/>
-      <c r="FS46" s="30"/>
+      <c r="FS46" s="118"/>
       <c r="FT46" s="30"/>
       <c r="FU46" s="30"/>
       <c r="FV46" s="30"/>
@@ -13074,23 +13105,20 @@
     </row>
     <row r="47" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="34"/>
-      <c r="B47" s="98" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="95" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" s="96">
-        <f>AVERAGE(D44:D46)</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="97">
-        <f>E44</f>
-        <v>45024</v>
-      </c>
-      <c r="F47" s="97">
-        <f>F46</f>
-        <v>45037</v>
+      <c r="B47" s="107" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="104"/>
+      <c r="D47" s="105">
+        <f>AVERAGE(D46,D40,D35)</f>
+        <v>0.50749999999999995</v>
+      </c>
+      <c r="E47" s="106">
+        <f>E27</f>
+        <v>44909</v>
+      </c>
+      <c r="F47" s="106">
+        <v>45048</v>
       </c>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
@@ -13260,7 +13288,7 @@
       <c r="FP47" s="30"/>
       <c r="FQ47" s="30"/>
       <c r="FR47" s="30"/>
-      <c r="FS47" s="30"/>
+      <c r="FS47" s="118"/>
       <c r="FT47" s="30"/>
       <c r="FU47" s="30"/>
       <c r="FV47" s="30"/>
@@ -13299,475 +13327,238 @@
       <c r="HC47" s="30"/>
     </row>
     <row r="48" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="34"/>
-      <c r="B48" s="115" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="112"/>
-      <c r="D48" s="113"/>
-      <c r="E48" s="114">
-        <f>E27</f>
-        <v>44909</v>
-      </c>
-      <c r="F48" s="114">
-        <v>45048</v>
-      </c>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
-      <c r="O48" s="30"/>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="30"/>
-      <c r="R48" s="30"/>
-      <c r="S48" s="30"/>
-      <c r="T48" s="30"/>
-      <c r="U48" s="30"/>
-      <c r="V48" s="30"/>
-      <c r="W48" s="30"/>
-      <c r="X48" s="30"/>
-      <c r="Y48" s="30"/>
-      <c r="Z48" s="30"/>
-      <c r="AA48" s="30"/>
-      <c r="AB48" s="30"/>
-      <c r="AC48" s="30"/>
-      <c r="AD48" s="30"/>
-      <c r="AE48" s="30"/>
-      <c r="AF48" s="30"/>
-      <c r="AG48" s="30"/>
-      <c r="AH48" s="30"/>
-      <c r="AI48" s="30"/>
-      <c r="AJ48" s="30"/>
-      <c r="AK48" s="30"/>
-      <c r="AL48" s="30"/>
-      <c r="AM48" s="30"/>
-      <c r="AN48" s="30"/>
-      <c r="AO48" s="30"/>
-      <c r="AP48" s="30"/>
-      <c r="AQ48" s="30"/>
-      <c r="AR48" s="30"/>
-      <c r="AS48" s="30"/>
-      <c r="AT48" s="30"/>
-      <c r="AU48" s="30"/>
-      <c r="AV48" s="30"/>
-      <c r="AW48" s="30"/>
-      <c r="AX48" s="30"/>
-      <c r="AY48" s="30"/>
-      <c r="AZ48" s="30"/>
-      <c r="BA48" s="30"/>
-      <c r="BB48" s="30"/>
-      <c r="BC48" s="30"/>
-      <c r="BD48" s="30"/>
-      <c r="BE48" s="30"/>
-      <c r="BF48" s="30"/>
-      <c r="BG48" s="30"/>
-      <c r="BH48" s="30"/>
-      <c r="BI48" s="30"/>
-      <c r="BJ48" s="30"/>
-      <c r="BK48" s="30"/>
-      <c r="BL48" s="30"/>
-      <c r="BM48" s="30"/>
-      <c r="BN48" s="101"/>
-      <c r="BO48" s="30"/>
-      <c r="BP48" s="30"/>
-      <c r="BQ48" s="30"/>
-      <c r="BR48" s="30"/>
-      <c r="BS48" s="30"/>
-      <c r="BT48" s="30"/>
-      <c r="BU48" s="30"/>
-      <c r="BV48" s="30"/>
-      <c r="BW48" s="30"/>
-      <c r="BX48" s="30"/>
-      <c r="BY48" s="30"/>
-      <c r="BZ48" s="30"/>
-      <c r="CA48" s="30"/>
-      <c r="CB48" s="30"/>
-      <c r="CC48" s="30"/>
-      <c r="CD48" s="30"/>
-      <c r="CE48" s="30"/>
-      <c r="CF48" s="30"/>
-      <c r="CG48" s="30"/>
-      <c r="CH48" s="30"/>
-      <c r="CI48" s="30"/>
-      <c r="CJ48" s="30"/>
-      <c r="CK48" s="30"/>
-      <c r="CL48" s="30"/>
-      <c r="CM48" s="30"/>
-      <c r="CN48" s="30"/>
-      <c r="CO48" s="30"/>
-      <c r="CP48" s="30"/>
-      <c r="CQ48" s="30"/>
-      <c r="CR48" s="30"/>
-      <c r="CS48" s="30"/>
-      <c r="CT48" s="30"/>
-      <c r="CU48" s="30"/>
-      <c r="CV48" s="30"/>
-      <c r="CW48" s="30"/>
-      <c r="CX48" s="30"/>
-      <c r="CY48" s="30"/>
-      <c r="CZ48" s="30"/>
-      <c r="DA48" s="30"/>
-      <c r="DB48" s="30"/>
-      <c r="DC48" s="30"/>
-      <c r="DD48" s="30"/>
-      <c r="DE48" s="30"/>
-      <c r="DF48" s="30"/>
-      <c r="DG48" s="30"/>
-      <c r="DH48" s="30"/>
-      <c r="DI48" s="30"/>
-      <c r="DJ48" s="30"/>
-      <c r="DK48" s="30"/>
-      <c r="DL48" s="30"/>
-      <c r="DM48" s="30"/>
-      <c r="DN48" s="30"/>
-      <c r="DO48" s="30"/>
-      <c r="DP48" s="30"/>
-      <c r="DQ48" s="30"/>
-      <c r="DR48" s="30"/>
-      <c r="DS48" s="30"/>
-      <c r="DT48" s="30"/>
-      <c r="DU48" s="30"/>
-      <c r="DV48" s="30"/>
-      <c r="DW48" s="30"/>
-      <c r="DX48" s="30"/>
-      <c r="DY48" s="30"/>
-      <c r="DZ48" s="30"/>
-      <c r="EA48" s="30"/>
-      <c r="EB48" s="30"/>
-      <c r="EC48" s="30"/>
-      <c r="ED48" s="30"/>
-      <c r="EE48" s="30"/>
-      <c r="EF48" s="30"/>
-      <c r="EG48" s="30"/>
-      <c r="EH48" s="30"/>
-      <c r="EI48" s="30"/>
-      <c r="EJ48" s="30"/>
-      <c r="EK48" s="30"/>
-      <c r="EL48" s="30"/>
-      <c r="EM48" s="30"/>
-      <c r="EN48" s="30"/>
-      <c r="EO48" s="30"/>
-      <c r="EP48" s="30"/>
-      <c r="EQ48" s="30"/>
-      <c r="ER48" s="30"/>
-      <c r="ES48" s="30"/>
-      <c r="ET48" s="30"/>
-      <c r="EU48" s="30"/>
-      <c r="EV48" s="30"/>
-      <c r="EW48" s="30"/>
-      <c r="EX48" s="30"/>
-      <c r="EY48" s="30"/>
-      <c r="EZ48" s="30"/>
-      <c r="FA48" s="30"/>
-      <c r="FB48" s="30"/>
-      <c r="FC48" s="30"/>
-      <c r="FD48" s="30"/>
-      <c r="FE48" s="30"/>
-      <c r="FF48" s="30"/>
-      <c r="FG48" s="30"/>
-      <c r="FH48" s="30"/>
-      <c r="FI48" s="30"/>
-      <c r="FJ48" s="30"/>
-      <c r="FK48" s="30"/>
-      <c r="FL48" s="30"/>
-      <c r="FM48" s="30"/>
-      <c r="FN48" s="30"/>
-      <c r="FO48" s="30"/>
-      <c r="FP48" s="30"/>
-      <c r="FQ48" s="30"/>
-      <c r="FR48" s="30"/>
-      <c r="FS48" s="30"/>
-      <c r="FT48" s="30"/>
-      <c r="FU48" s="30"/>
-      <c r="FV48" s="30"/>
-      <c r="FW48" s="30"/>
-      <c r="FX48" s="30"/>
-      <c r="FY48" s="30"/>
-      <c r="FZ48" s="30"/>
-      <c r="GA48" s="30"/>
-      <c r="GB48" s="30"/>
-      <c r="GC48" s="30"/>
-      <c r="GD48" s="30"/>
-      <c r="GE48" s="30"/>
-      <c r="GF48" s="30"/>
-      <c r="GG48" s="30"/>
-      <c r="GH48" s="30"/>
-      <c r="GI48" s="30"/>
-      <c r="GJ48" s="30"/>
-      <c r="GK48" s="30"/>
-      <c r="GL48" s="30"/>
-      <c r="GM48" s="30"/>
-      <c r="GN48" s="30"/>
-      <c r="GO48" s="30"/>
-      <c r="GP48" s="30"/>
-      <c r="GQ48" s="30"/>
-      <c r="GR48" s="30"/>
-      <c r="GS48" s="30"/>
-      <c r="GT48" s="30"/>
-      <c r="GU48" s="30"/>
-      <c r="GV48" s="30"/>
-      <c r="GW48" s="30"/>
-      <c r="GX48" s="75"/>
-      <c r="GY48" s="30"/>
-      <c r="GZ48" s="30"/>
-      <c r="HA48" s="30"/>
-      <c r="HB48" s="30"/>
-      <c r="HC48" s="30"/>
-    </row>
-    <row r="49" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C49" s="27"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="69"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29" t="str">
+      <c r="A48" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="27"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="68"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29" t="str">
         <f t="shared" si="143"/>
         <v/>
       </c>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="32"/>
-      <c r="R49" s="32"/>
-      <c r="S49" s="32"/>
-      <c r="T49" s="32"/>
-      <c r="U49" s="32"/>
-      <c r="V49" s="32"/>
-      <c r="W49" s="32"/>
-      <c r="X49" s="32"/>
-      <c r="Y49" s="32"/>
-      <c r="Z49" s="32"/>
-      <c r="AA49" s="32"/>
-      <c r="AB49" s="32"/>
-      <c r="AC49" s="32"/>
-      <c r="AD49" s="32"/>
-      <c r="AE49" s="32"/>
-      <c r="AF49" s="32"/>
-      <c r="AG49" s="32"/>
-      <c r="AH49" s="32"/>
-      <c r="AI49" s="32"/>
-      <c r="AJ49" s="32"/>
-      <c r="AK49" s="32"/>
-      <c r="AL49" s="32"/>
-      <c r="AM49" s="32"/>
-      <c r="AN49" s="32"/>
-      <c r="AO49" s="32"/>
-      <c r="AP49" s="32"/>
-      <c r="AQ49" s="32"/>
-      <c r="AR49" s="32"/>
-      <c r="AS49" s="32"/>
-      <c r="AT49" s="32"/>
-      <c r="AU49" s="32"/>
-      <c r="AV49" s="32"/>
-      <c r="AW49" s="32"/>
-      <c r="AX49" s="32"/>
-      <c r="AY49" s="32"/>
-      <c r="AZ49" s="32"/>
-      <c r="BA49" s="32"/>
-      <c r="BB49" s="32"/>
-      <c r="BC49" s="32"/>
-      <c r="BD49" s="32"/>
-      <c r="BE49" s="32"/>
-      <c r="BF49" s="32"/>
-      <c r="BG49" s="32"/>
-      <c r="BH49" s="32"/>
-      <c r="BI49" s="32"/>
-      <c r="BJ49" s="32"/>
-      <c r="BK49" s="32"/>
-      <c r="BL49" s="32"/>
-      <c r="BM49" s="32"/>
-      <c r="BN49" s="101"/>
-      <c r="BO49" s="32"/>
-      <c r="BP49" s="32"/>
-      <c r="BQ49" s="32"/>
-      <c r="BR49" s="32"/>
-      <c r="BS49" s="32"/>
-      <c r="BT49" s="32"/>
-      <c r="BU49" s="32"/>
-      <c r="BV49" s="32"/>
-      <c r="BW49" s="32"/>
-      <c r="BX49" s="32"/>
-      <c r="BY49" s="32"/>
-      <c r="BZ49" s="32"/>
-      <c r="CA49" s="32"/>
-      <c r="CB49" s="32"/>
-      <c r="CC49" s="32"/>
-      <c r="CD49" s="32"/>
-      <c r="CE49" s="32"/>
-      <c r="CF49" s="32"/>
-      <c r="CG49" s="32"/>
-      <c r="CH49" s="32"/>
-      <c r="CI49" s="32"/>
-      <c r="CJ49" s="32"/>
-      <c r="CK49" s="32"/>
-      <c r="CL49" s="32"/>
-      <c r="CM49" s="32"/>
-      <c r="CN49" s="32"/>
-      <c r="CO49" s="32"/>
-      <c r="CP49" s="32"/>
-      <c r="CQ49" s="32"/>
-      <c r="CR49" s="32"/>
-      <c r="CS49" s="32"/>
-      <c r="CT49" s="32"/>
-      <c r="CU49" s="32"/>
-      <c r="CV49" s="32"/>
-      <c r="CW49" s="32"/>
-      <c r="CX49" s="32"/>
-      <c r="CY49" s="32"/>
-      <c r="CZ49" s="32"/>
-      <c r="DA49" s="32"/>
-      <c r="DB49" s="32"/>
-      <c r="DC49" s="32"/>
-      <c r="DD49" s="32"/>
-      <c r="DE49" s="32"/>
-      <c r="DF49" s="32"/>
-      <c r="DG49" s="32"/>
-      <c r="DH49" s="32"/>
-      <c r="DI49" s="32"/>
-      <c r="DJ49" s="32"/>
-      <c r="DK49" s="32"/>
-      <c r="DL49" s="32"/>
-      <c r="DM49" s="32"/>
-      <c r="DN49" s="32"/>
-      <c r="DO49" s="32"/>
-      <c r="DP49" s="32"/>
-      <c r="DQ49" s="32"/>
-      <c r="DR49" s="32"/>
-      <c r="DS49" s="32"/>
-      <c r="DT49" s="32"/>
-      <c r="DU49" s="32"/>
-      <c r="DV49" s="32"/>
-      <c r="DW49" s="32"/>
-      <c r="DX49" s="32"/>
-      <c r="DY49" s="32"/>
-      <c r="DZ49" s="32"/>
-      <c r="EA49" s="32"/>
-      <c r="EB49" s="32"/>
-      <c r="EC49" s="32"/>
-      <c r="ED49" s="32"/>
-      <c r="EE49" s="32"/>
-      <c r="EF49" s="32"/>
-      <c r="EG49" s="32"/>
-      <c r="EH49" s="32"/>
-      <c r="EI49" s="32"/>
-      <c r="EJ49" s="32"/>
-      <c r="EK49" s="32"/>
-      <c r="EL49" s="32"/>
-      <c r="EM49" s="32"/>
-      <c r="EN49" s="32"/>
-      <c r="EO49" s="32"/>
-      <c r="EP49" s="32"/>
-      <c r="EQ49" s="32"/>
-      <c r="ER49" s="32"/>
-      <c r="ES49" s="32"/>
-      <c r="ET49" s="32"/>
-      <c r="EU49" s="32"/>
-      <c r="EV49" s="32"/>
-      <c r="EW49" s="32"/>
-      <c r="EX49" s="32"/>
-      <c r="EY49" s="32"/>
-      <c r="EZ49" s="32"/>
-      <c r="FA49" s="32"/>
-      <c r="FB49" s="32"/>
-      <c r="FC49" s="32"/>
-      <c r="FD49" s="32"/>
-      <c r="FE49" s="32"/>
-      <c r="FF49" s="32"/>
-      <c r="FG49" s="32"/>
-      <c r="FH49" s="32"/>
-      <c r="FI49" s="32"/>
-      <c r="FJ49" s="32"/>
-      <c r="FK49" s="32"/>
-      <c r="FL49" s="32"/>
-      <c r="FM49" s="32"/>
-      <c r="FN49" s="32"/>
-      <c r="FO49" s="32"/>
-      <c r="FP49" s="32"/>
-      <c r="FQ49" s="32"/>
-      <c r="FR49" s="32"/>
-      <c r="FS49" s="32"/>
-      <c r="FT49" s="32"/>
-      <c r="FU49" s="32"/>
-      <c r="FV49" s="32"/>
-      <c r="FW49" s="32"/>
-      <c r="FX49" s="32"/>
-      <c r="FY49" s="32"/>
-      <c r="FZ49" s="32"/>
-      <c r="GA49" s="32"/>
-      <c r="GB49" s="32"/>
-      <c r="GC49" s="32"/>
-      <c r="GD49" s="32"/>
-      <c r="GE49" s="32"/>
-      <c r="GF49" s="32"/>
-      <c r="GG49" s="32"/>
-      <c r="GH49" s="32"/>
-      <c r="GI49" s="32"/>
-      <c r="GJ49" s="32"/>
-      <c r="GK49" s="32"/>
-      <c r="GL49" s="32"/>
-      <c r="GM49" s="32"/>
-      <c r="GN49" s="32"/>
-      <c r="GO49" s="32"/>
-      <c r="GP49" s="32"/>
-      <c r="GQ49" s="32"/>
-      <c r="GR49" s="32"/>
-      <c r="GS49" s="32"/>
-      <c r="GT49" s="32"/>
-      <c r="GU49" s="32"/>
-      <c r="GV49" s="32"/>
-      <c r="GW49" s="32"/>
-      <c r="GX49" s="75"/>
-      <c r="GY49" s="32"/>
-      <c r="GZ49" s="32"/>
-      <c r="HA49" s="32"/>
-      <c r="HB49" s="32"/>
-      <c r="HC49" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="32"/>
+      <c r="N48" s="32"/>
+      <c r="O48" s="32"/>
+      <c r="P48" s="32"/>
+      <c r="Q48" s="32"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="32"/>
+      <c r="V48" s="32"/>
+      <c r="W48" s="32"/>
+      <c r="X48" s="32"/>
+      <c r="Y48" s="32"/>
+      <c r="Z48" s="32"/>
+      <c r="AA48" s="32"/>
+      <c r="AB48" s="32"/>
+      <c r="AC48" s="32"/>
+      <c r="AD48" s="32"/>
+      <c r="AE48" s="32"/>
+      <c r="AF48" s="32"/>
+      <c r="AG48" s="32"/>
+      <c r="AH48" s="32"/>
+      <c r="AI48" s="32"/>
+      <c r="AJ48" s="32"/>
+      <c r="AK48" s="32"/>
+      <c r="AL48" s="32"/>
+      <c r="AM48" s="32"/>
+      <c r="AN48" s="32"/>
+      <c r="AO48" s="32"/>
+      <c r="AP48" s="32"/>
+      <c r="AQ48" s="32"/>
+      <c r="AR48" s="32"/>
+      <c r="AS48" s="32"/>
+      <c r="AT48" s="32"/>
+      <c r="AU48" s="32"/>
+      <c r="AV48" s="32"/>
+      <c r="AW48" s="32"/>
+      <c r="AX48" s="32"/>
+      <c r="AY48" s="32"/>
+      <c r="AZ48" s="32"/>
+      <c r="BA48" s="32"/>
+      <c r="BB48" s="32"/>
+      <c r="BC48" s="32"/>
+      <c r="BD48" s="32"/>
+      <c r="BE48" s="32"/>
+      <c r="BF48" s="32"/>
+      <c r="BG48" s="32"/>
+      <c r="BH48" s="32"/>
+      <c r="BI48" s="32"/>
+      <c r="BJ48" s="32"/>
+      <c r="BK48" s="32"/>
+      <c r="BL48" s="32"/>
+      <c r="BM48" s="32"/>
+      <c r="BN48" s="101"/>
+      <c r="BO48" s="32"/>
+      <c r="BP48" s="32"/>
+      <c r="BQ48" s="32"/>
+      <c r="BR48" s="32"/>
+      <c r="BS48" s="32"/>
+      <c r="BT48" s="32"/>
+      <c r="BU48" s="32"/>
+      <c r="BV48" s="32"/>
+      <c r="BW48" s="32"/>
+      <c r="BX48" s="32"/>
+      <c r="BY48" s="32"/>
+      <c r="BZ48" s="32"/>
+      <c r="CA48" s="32"/>
+      <c r="CB48" s="32"/>
+      <c r="CC48" s="32"/>
+      <c r="CD48" s="32"/>
+      <c r="CE48" s="32"/>
+      <c r="CF48" s="32"/>
+      <c r="CG48" s="32"/>
+      <c r="CH48" s="32"/>
+      <c r="CI48" s="32"/>
+      <c r="CJ48" s="32"/>
+      <c r="CK48" s="32"/>
+      <c r="CL48" s="32"/>
+      <c r="CM48" s="32"/>
+      <c r="CN48" s="32"/>
+      <c r="CO48" s="32"/>
+      <c r="CP48" s="32"/>
+      <c r="CQ48" s="32"/>
+      <c r="CR48" s="32"/>
+      <c r="CS48" s="32"/>
+      <c r="CT48" s="32"/>
+      <c r="CU48" s="32"/>
+      <c r="CV48" s="32"/>
+      <c r="CW48" s="32"/>
+      <c r="CX48" s="32"/>
+      <c r="CY48" s="32"/>
+      <c r="CZ48" s="32"/>
+      <c r="DA48" s="32"/>
+      <c r="DB48" s="32"/>
+      <c r="DC48" s="32"/>
+      <c r="DD48" s="32"/>
+      <c r="DE48" s="32"/>
+      <c r="DF48" s="32"/>
+      <c r="DG48" s="32"/>
+      <c r="DH48" s="32"/>
+      <c r="DI48" s="32"/>
+      <c r="DJ48" s="32"/>
+      <c r="DK48" s="32"/>
+      <c r="DL48" s="32"/>
+      <c r="DM48" s="32"/>
+      <c r="DN48" s="32"/>
+      <c r="DO48" s="32"/>
+      <c r="DP48" s="32"/>
+      <c r="DQ48" s="32"/>
+      <c r="DR48" s="32"/>
+      <c r="DS48" s="32"/>
+      <c r="DT48" s="32"/>
+      <c r="DU48" s="32"/>
+      <c r="DV48" s="32"/>
+      <c r="DW48" s="32"/>
+      <c r="DX48" s="32"/>
+      <c r="DY48" s="32"/>
+      <c r="DZ48" s="32"/>
+      <c r="EA48" s="32"/>
+      <c r="EB48" s="32"/>
+      <c r="EC48" s="32"/>
+      <c r="ED48" s="32"/>
+      <c r="EE48" s="32"/>
+      <c r="EF48" s="32"/>
+      <c r="EG48" s="32"/>
+      <c r="EH48" s="32"/>
+      <c r="EI48" s="32"/>
+      <c r="EJ48" s="32"/>
+      <c r="EK48" s="32"/>
+      <c r="EL48" s="32"/>
+      <c r="EM48" s="32"/>
+      <c r="EN48" s="32"/>
+      <c r="EO48" s="32"/>
+      <c r="EP48" s="32"/>
+      <c r="EQ48" s="32"/>
+      <c r="ER48" s="32"/>
+      <c r="ES48" s="32"/>
+      <c r="ET48" s="32"/>
+      <c r="EU48" s="32"/>
+      <c r="EV48" s="32"/>
+      <c r="EW48" s="32"/>
+      <c r="EX48" s="32"/>
+      <c r="EY48" s="32"/>
+      <c r="EZ48" s="32"/>
+      <c r="FA48" s="32"/>
+      <c r="FB48" s="32"/>
+      <c r="FC48" s="32"/>
+      <c r="FD48" s="32"/>
+      <c r="FE48" s="32"/>
+      <c r="FF48" s="32"/>
+      <c r="FG48" s="32"/>
+      <c r="FH48" s="32"/>
+      <c r="FI48" s="32"/>
+      <c r="FJ48" s="32"/>
+      <c r="FK48" s="32"/>
+      <c r="FL48" s="32"/>
+      <c r="FM48" s="32"/>
+      <c r="FN48" s="32"/>
+      <c r="FO48" s="32"/>
+      <c r="FP48" s="32"/>
+      <c r="FQ48" s="32"/>
+      <c r="FR48" s="32"/>
+      <c r="FS48" s="118"/>
+      <c r="FT48" s="32"/>
+      <c r="FU48" s="32"/>
+      <c r="FV48" s="32"/>
+      <c r="FW48" s="32"/>
+      <c r="FX48" s="32"/>
+      <c r="FY48" s="32"/>
+      <c r="FZ48" s="32"/>
+      <c r="GA48" s="32"/>
+      <c r="GB48" s="32"/>
+      <c r="GC48" s="32"/>
+      <c r="GD48" s="32"/>
+      <c r="GE48" s="32"/>
+      <c r="GF48" s="32"/>
+      <c r="GG48" s="32"/>
+      <c r="GH48" s="32"/>
+      <c r="GI48" s="32"/>
+      <c r="GJ48" s="32"/>
+      <c r="GK48" s="32"/>
+      <c r="GL48" s="32"/>
+      <c r="GM48" s="32"/>
+      <c r="GN48" s="32"/>
+      <c r="GO48" s="32"/>
+      <c r="GP48" s="32"/>
+      <c r="GQ48" s="32"/>
+      <c r="GR48" s="32"/>
+      <c r="GS48" s="32"/>
+      <c r="GT48" s="32"/>
+      <c r="GU48" s="32"/>
+      <c r="GV48" s="32"/>
+      <c r="GW48" s="32"/>
+      <c r="GX48" s="75"/>
+      <c r="GY48" s="32"/>
+      <c r="GZ48" s="32"/>
+      <c r="HA48" s="32"/>
+      <c r="HB48" s="32"/>
+      <c r="HC48" s="32"/>
     </row>
-    <row r="50" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G50" s="6"/>
+    <row r="49" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G49" s="6"/>
     </row>
-    <row r="51" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C51" s="11"/>
-      <c r="F51" s="36"/>
+    <row r="50" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="11"/>
+      <c r="F50" s="36"/>
     </row>
-    <row r="52" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="12"/>
+    <row r="51" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="FN4:FT4"/>
-    <mergeCell ref="FU4:GA4"/>
-    <mergeCell ref="GB4:GH4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
+  <mergeCells count="35">
+    <mergeCell ref="FS2:GF2"/>
     <mergeCell ref="GX2:HD2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -13784,9 +13575,27 @@
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="DJ4:DP4"/>
     <mergeCell ref="BN2:BS2"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="GI4:GO4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="FG4:FM4"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="FU4:GA4"/>
+    <mergeCell ref="GB4:GH4"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D11 D49 D13:D14 D28:D34 D16:D26">
+  <conditionalFormatting sqref="D7:D11 D13:D14 D16:D26 D28:D48">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13800,31 +13609,17 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:HC49">
+  <conditionalFormatting sqref="I5:HC48">
     <cfRule type="expression" dxfId="3" priority="34">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:HC49">
+  <conditionalFormatting sqref="I7:HC48">
     <cfRule type="expression" dxfId="2" priority="20">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="33" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D48">
-    <cfRule type="dataBar" priority="4">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{43BDC079-A4D3-4950-81E9-81F0EA5236AE}</x14:id>
-        </ext>
-      </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
@@ -13869,7 +13664,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN5:BN49">
+  <conditionalFormatting sqref="BN5:BN48">
     <cfRule type="expression" dxfId="0" priority="39">
       <formula>TRUE</formula>
     </cfRule>
@@ -13901,22 +13696,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D11 D49 D13:D14 D28:D34 D16:D26</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{43BDC079-A4D3-4950-81E9-81F0EA5236AE}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D35:D48</xm:sqref>
+          <xm:sqref>D7:D11 D13:D14 D16:D26 D28:D48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C5B9DC40-6AA5-4EDE-985B-6615ABEB3CA0}">
@@ -13970,6 +13750,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="ade9cf8d-689b-44c7-83d3-1b6d2ed01456" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD32B88E8F5C5840BE58EFBF8C533A84" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eefc930e7d3d41296f1e209179b210f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ade9cf8d-689b-44c7-83d3-1b6d2ed01456" xmlns:ns4="f2c43e5f-0c15-4f9b-b257-1465459d1450" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9fa27b00dd7b8e982819c8d20ed7c1fa" ns3:_="" ns4:_="">
     <xsd:import namespace="ade9cf8d-689b-44c7-83d3-1b6d2ed01456"/>
@@ -14172,24 +13969,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="f2c43e5f-0c15-4f9b-b257-1465459d1450"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ade9cf8d-689b-44c7-83d3-1b6d2ed01456"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="ade9cf8d-689b-44c7-83d3-1b6d2ed01456" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB27BE46-3210-44BF-89A8-85069933A938}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14206,29 +14011,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f2c43e5f-0c15-4f9b-b257-1465459d1450"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ade9cf8d-689b-44c7-83d3-1b6d2ed01456"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>